<commit_message>
Added more improvements to Excel connector
</commit_message>
<xml_diff>
--- a/tst/Encamina.Enmarcha.SemanticKernel.Connectors.Document.Tests/TestUtilities/Files/TestFile.xlsx
+++ b/tst/Encamina.Enmarcha.SemanticKernel.Connectors.Document.Tests/TestUtilities/Files/TestFile.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lmarcos\source\repos\ConsoleApp1\TestProject1\TestUtilities\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lmarcos\OneDrive - ENCAMINA S.L\Documentos\GitHub\enmarcha\tst\Encamina.Enmarcha.SemanticKernel.Connectors.Document.Tests\TestUtilities\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75186E28-F18D-4363-B8A3-C8B65E9B99EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41004879-C306-45DC-BA6C-CFA1714D3627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="51480" yWindow="2850" windowWidth="29040" windowHeight="15720" xr2:uid="{C925E0C8-F8E3-4EA1-B7AA-7F277CE8249A}"/>
   </bookViews>
@@ -78,8 +78,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,7 +398,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A3" sqref="A3:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -408,35 +409,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>11</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>12</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>13</v>
       </c>
     </row>

</xml_diff>